<commit_message>
update the GB -> UK adjusting of gambling and alcohol expenditure data
</commit_message>
<xml_diff>
--- a/data-raw/data/Disaggregated_tax_and_NICs_receipts_-_statistics_table.xlsx
+++ b/data-raw/data/Disaggregated_tax_and_NICs_receipts_-_statistics_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\PHEDS\Research Attachments\InputOutput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\HAR_PR\PR\InputOutput\Code\models\cdohio.mod\data-raw\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D81EC060-D9F6-470E-A11B-69074C858C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A1E6B67A-00AF-4A68-8AE9-F0699C3E7961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="1740" windowWidth="14400" windowHeight="7360"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final_values" sheetId="1" r:id="rId1"/>
@@ -338,10 +338,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0;&quot;-&quot;#,##0;&quot;-  &quot;;@"/>
     <numFmt numFmtId="165" formatCode="0.0%;&quot;-&quot;0.0%;&quot;-  &quot;;@"/>
+    <numFmt numFmtId="172" formatCode="0.0%"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -399,7 +400,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -409,6 +410,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -459,7 +472,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -497,6 +510,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -812,28 +831,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="P149" workbookViewId="0">
+      <selection activeCell="V159" sqref="V159"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="5" customWidth="1"/>
-    <col min="2" max="32" width="14.09765625" style="2" customWidth="1"/>
-    <col min="33" max="33" width="14.09765625" style="3" customWidth="1"/>
-    <col min="34" max="39" width="14.09765625" style="2" customWidth="1"/>
-    <col min="40" max="40" width="9.3984375" style="4" customWidth="1"/>
-    <col min="41" max="16384" width="9.3984375" style="4"/>
+    <col min="1" max="1" width="16.44140625" style="5" customWidth="1"/>
+    <col min="2" max="32" width="14.109375" style="2" customWidth="1"/>
+    <col min="33" max="33" width="14.109375" style="3" customWidth="1"/>
+    <col min="34" max="39" width="14.109375" style="2" customWidth="1"/>
+    <col min="40" max="40" width="9.44140625" style="4" customWidth="1"/>
+    <col min="41" max="16384" width="9.44140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:39" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:39" s="5" customFormat="1" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:39" s="5" customFormat="1" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -3290,7 +3311,7 @@
         <v>11551.739419909998</v>
       </c>
     </row>
-    <row r="24" spans="1:39" s="11" customFormat="1" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:39" s="11" customFormat="1" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
@@ -8127,7 +8148,7 @@
         <v>9772.5083228754011</v>
       </c>
     </row>
-    <row r="66" spans="1:39" s="5" customFormat="1" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:39" s="5" customFormat="1" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>66</v>
       </c>
@@ -12964,7 +12985,7 @@
         <v>548.36536602871274</v>
       </c>
     </row>
-    <row r="108" spans="1:39" s="13" customFormat="1" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:39" s="13" customFormat="1" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A108" s="1" t="s">
         <v>67</v>
       </c>
@@ -17801,7 +17822,7 @@
         <v>845.52437811181721</v>
       </c>
     </row>
-    <row r="150" spans="1:39" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="150" spans="1:39" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A150" s="6" t="s">
         <v>68</v>
       </c>
@@ -19854,22 +19875,22 @@
       <c r="U167" s="12">
         <v>6.2669802961655367E-3</v>
       </c>
-      <c r="V167" s="12">
+      <c r="V167" s="18">
         <v>5.0906587528258176E-2</v>
       </c>
-      <c r="W167" s="12">
+      <c r="W167" s="18">
         <v>3.6667646182520518E-2</v>
       </c>
-      <c r="X167" s="12">
+      <c r="X167" s="18">
         <v>2.8465450319318481E-2</v>
       </c>
-      <c r="Y167" s="12">
+      <c r="Y167" s="18">
         <v>2.2667510360526465E-2</v>
       </c>
-      <c r="Z167" s="12">
+      <c r="Z167" s="18">
         <v>2.1414798146675688E-2</v>
       </c>
-      <c r="AA167" s="12">
+      <c r="AA167" s="18">
         <v>3.7908913305529771E-2</v>
       </c>
       <c r="AB167" s="12">
@@ -19971,22 +19992,22 @@
       <c r="U168" s="12">
         <v>5.3174971241270637E-3</v>
       </c>
-      <c r="V168" s="12">
+      <c r="V168" s="18">
         <v>5.6533954635784277E-2</v>
       </c>
-      <c r="W168" s="12">
+      <c r="W168" s="18">
         <v>3.8064459623191563E-2</v>
       </c>
-      <c r="X168" s="12">
+      <c r="X168" s="18">
         <v>2.8668374305898574E-2</v>
       </c>
-      <c r="Y168" s="12">
+      <c r="Y168" s="18">
         <v>2.3654400327425138E-2</v>
       </c>
-      <c r="Z168" s="12">
+      <c r="Z168" s="18">
         <v>2.2187025337467723E-2</v>
       </c>
-      <c r="AA168" s="12">
+      <c r="AA168" s="18">
         <v>3.7831021437578813E-2</v>
       </c>
       <c r="AB168" s="12">
@@ -20088,22 +20109,22 @@
       <c r="U169" s="12">
         <v>4.953034369725536E-3</v>
       </c>
-      <c r="V169" s="12">
+      <c r="V169" s="18">
         <v>5.8776846386587964E-2</v>
       </c>
-      <c r="W169" s="12">
+      <c r="W169" s="18">
         <v>3.7829156607330904E-2</v>
       </c>
-      <c r="X169" s="12">
+      <c r="X169" s="18">
         <v>2.5113157046004371E-2</v>
       </c>
-      <c r="Y169" s="12">
+      <c r="Y169" s="18">
         <v>2.435964382578051E-2</v>
       </c>
-      <c r="Z169" s="12">
+      <c r="Z169" s="18">
         <v>1.6983953156213094E-2</v>
       </c>
-      <c r="AA169" s="12">
+      <c r="AA169" s="18">
         <v>3.5091310514233913E-2</v>
       </c>
       <c r="AB169" s="12">
@@ -20205,22 +20226,22 @@
       <c r="U170" s="12">
         <v>4.7736519745437351E-3</v>
       </c>
-      <c r="V170" s="12">
+      <c r="V170" s="18">
         <v>5.8776846386587964E-2</v>
       </c>
-      <c r="W170" s="12">
+      <c r="W170" s="18">
         <v>3.7829156607330904E-2</v>
       </c>
-      <c r="X170" s="12">
+      <c r="X170" s="18">
         <v>2.5113157046004371E-2</v>
       </c>
-      <c r="Y170" s="12">
+      <c r="Y170" s="18">
         <v>2.435964382578051E-2</v>
       </c>
-      <c r="Z170" s="12">
+      <c r="Z170" s="18">
         <v>1.6983953156213094E-2</v>
       </c>
-      <c r="AA170" s="12">
+      <c r="AA170" s="18">
         <v>3.5091310514233913E-2</v>
       </c>
       <c r="AB170" s="12">
@@ -20280,12 +20301,30 @@
       <c r="S171" s="10"/>
       <c r="T171" s="10"/>
       <c r="U171" s="10"/>
-      <c r="V171" s="10"/>
-      <c r="W171" s="10"/>
-      <c r="X171" s="10"/>
-      <c r="Y171" s="10"/>
-      <c r="Z171" s="10"/>
-      <c r="AA171" s="10"/>
+      <c r="V171" s="19">
+        <f t="shared" ref="V171:Z171" si="0">AVERAGE(V167:V170)</f>
+        <v>5.6248558734304593E-2</v>
+      </c>
+      <c r="W171" s="19">
+        <f t="shared" si="0"/>
+        <v>3.7597604755093474E-2</v>
+      </c>
+      <c r="X171" s="19">
+        <f t="shared" si="0"/>
+        <v>2.684003467930645E-2</v>
+      </c>
+      <c r="Y171" s="19">
+        <f t="shared" si="0"/>
+        <v>2.3760299584878158E-2</v>
+      </c>
+      <c r="Z171" s="19">
+        <f t="shared" si="0"/>
+        <v>1.9392432449142398E-2</v>
+      </c>
+      <c r="AA171" s="19">
+        <f>AVERAGE(AA167:AA170)</f>
+        <v>3.6480638942894106E-2</v>
+      </c>
       <c r="AB171" s="10"/>
       <c r="AC171" s="10"/>
       <c r="AD171" s="10"/>
@@ -22521,7 +22560,7 @@
         <v>386.38463820338228</v>
       </c>
     </row>
-    <row r="191" spans="1:39" ht="13" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A191" s="9" t="s">
         <v>58</v>
       </c>
@@ -22638,8 +22677,7 @@
         <v>385.34135289406561</v>
       </c>
     </row>
-    <row r="192" spans="1:39" ht="13" x14ac:dyDescent="0.3"/>
-    <row r="193" spans="1:39" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:39" ht="15" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
         <v>70</v>
       </c>
@@ -22687,7 +22725,7 @@
       <c r="AL194" s="16"/>
       <c r="AM194" s="16"/>
     </row>
-    <row r="195" spans="1:39" ht="13" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A195" s="17"/>
       <c r="B195" s="17"/>
       <c r="C195" s="17"/>
@@ -22728,7 +22766,7 @@
       <c r="AL195" s="16"/>
       <c r="AM195" s="16"/>
     </row>
-    <row r="196" spans="1:39" ht="13" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A196" s="17"/>
       <c r="B196" s="17"/>
       <c r="C196" s="17"/>
@@ -22769,12 +22807,12 @@
       <c r="AL196" s="16"/>
       <c r="AM196" s="16"/>
     </row>
-    <row r="197" spans="1:39" ht="13" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A197" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="198" spans="1:39" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:39" ht="15" x14ac:dyDescent="0.3">
       <c r="A198" s="5" t="s">
         <v>73</v>
       </c>

</xml_diff>